<commit_message>
viel Events und Notifications zwischen Controller-Data und Controller-HD hergestellt versucht, combobox einzubinden.
</commit_message>
<xml_diff>
--- a/ShadowRun_Charakter_Helper/ShadowRun_Charakter_Helper/Hilfe.xlsx
+++ b/ShadowRun_Charakter_Helper/ShadowRun_Charakter_Helper/Hilfe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="0" windowWidth="26805" windowHeight="12195"/>
+    <workbookView xWindow="3990" yWindow="0" windowWidth="26805" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="24">
   <si>
     <t>Handlung</t>
   </si>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:P27"/>
+  <dimension ref="C1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22:P27"/>
+      <selection activeCell="V27" sqref="V22:V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +431,7 @@
     <col min="10" max="10" width="81.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>17</v>
       </c>
@@ -447,8 +447,14 @@
       <c r="O1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>16</v>
       </c>
@@ -464,8 +470,14 @@
       <c r="O2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D3" t="str">
         <f>"public ObservableCollection&lt;CharController."</f>
         <v>public ObservableCollection&lt;CharController.</v>
@@ -489,8 +501,14 @@
       <c r="P3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D4" t="str">
         <f>"&gt; "</f>
         <v xml:space="preserve">&gt; </v>
@@ -522,8 +540,21 @@
       <c r="P4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" t="str">
+        <f>"Controller = "</f>
+        <v xml:space="preserve">Controller = </v>
+      </c>
+      <c r="V4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D5" t="str">
         <f>"Controller { get; set; }"</f>
         <v>Controller { get; set; }</v>
@@ -555,8 +586,22 @@
       <c r="P5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R5" t="str">
+        <f>","</f>
+        <v>,</v>
+      </c>
+      <c r="S5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" t="str">
+        <f>"Controller;"</f>
+        <v>Controller;</v>
+      </c>
+      <c r="V5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -572,8 +617,14 @@
       <c r="P6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -608,8 +659,22 @@
       <c r="O7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" t="str">
+        <f>R$3&amp;$C7&amp;R$4&amp;R$5</f>
+        <v>HandlungController,</v>
+      </c>
+      <c r="U7" t="s">
+        <v>20</v>
+      </c>
+      <c r="V7" t="str">
+        <f>U$3&amp;$C7&amp;U$4&amp;LOWER($C7)&amp;U$5</f>
+        <v>HandlungController = handlungController;</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>1</v>
       </c>
@@ -644,8 +709,22 @@
       <c r="O8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" ref="S8:S16" si="4">R$3&amp;$C8&amp;R$4&amp;R$5</f>
+        <v>FertigkeitController,</v>
+      </c>
+      <c r="U8" t="s">
+        <v>20</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" ref="V8:V16" si="5">U$3&amp;$C8&amp;U$4&amp;LOWER($C8)&amp;U$5</f>
+        <v>FertigkeitController = fertigkeitController;</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -680,8 +759,22 @@
       <c r="O9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="4"/>
+        <v>AttributController,</v>
+      </c>
+      <c r="U9" t="s">
+        <v>20</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="5"/>
+        <v>AttributController = attributController;</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>3</v>
       </c>
@@ -716,8 +809,22 @@
       <c r="O10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="4"/>
+        <v>ItemController,</v>
+      </c>
+      <c r="U10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="5"/>
+        <v>ItemController = itemController;</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>4</v>
       </c>
@@ -752,8 +859,22 @@
       <c r="O11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="4"/>
+        <v>MunitionController,</v>
+      </c>
+      <c r="U11" t="s">
+        <v>20</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="5"/>
+        <v>MunitionController = munitionController;</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>5</v>
       </c>
@@ -788,8 +909,22 @@
       <c r="O12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="4"/>
+        <v>ImplantatController,</v>
+      </c>
+      <c r="U12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="5"/>
+        <v>ImplantatController = implantatController;</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -824,8 +959,22 @@
       <c r="O13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="4"/>
+        <v>VorteilController,</v>
+      </c>
+      <c r="U13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="5"/>
+        <v>VorteilController = vorteilController;</v>
+      </c>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -860,8 +1009,22 @@
       <c r="O14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R14" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="4"/>
+        <v>NachteilController,</v>
+      </c>
+      <c r="U14" t="s">
+        <v>20</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="5"/>
+        <v>NachteilController = nachteilController;</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>8</v>
       </c>
@@ -896,8 +1059,22 @@
       <c r="O15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
+        <v>20</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="4"/>
+        <v>ConnectionController,</v>
+      </c>
+      <c r="U15" t="s">
+        <v>20</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="5"/>
+        <v>ConnectionController = connectionController;</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -932,8 +1109,22 @@
       <c r="O16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>20</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" si="4"/>
+        <v>SinController,</v>
+      </c>
+      <c r="U16" t="s">
+        <v>20</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="5"/>
+        <v>SinController = sinController;</v>
+      </c>
+    </row>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>20</v>
       </c>
@@ -961,8 +1152,20 @@
       <c r="O17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>20</v>
+      </c>
+      <c r="S17" t="s">
+        <v>20</v>
+      </c>
+      <c r="U17" t="s">
+        <v>20</v>
+      </c>
+      <c r="V17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f>"public CharController."</f>
         <v>public CharController.</v>
@@ -989,8 +1192,14 @@
       <c r="P18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>20</v>
+      </c>
+      <c r="V18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f>" "</f>
         <v xml:space="preserve"> </v>
@@ -1027,8 +1236,21 @@
       <c r="P19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>23</v>
+      </c>
+      <c r="S19" t="s">
+        <v>20</v>
+      </c>
+      <c r="U19" t="str">
+        <f>"Controller = "</f>
+        <v xml:space="preserve">Controller = </v>
+      </c>
+      <c r="V19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f>"Controller { get; set; }"</f>
         <v>Controller { get; set; }</v>
@@ -1067,8 +1289,22 @@
       <c r="P20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R20" t="str">
+        <f>","</f>
+        <v>,</v>
+      </c>
+      <c r="S20" t="s">
+        <v>20</v>
+      </c>
+      <c r="U20" t="str">
+        <f>"Controller;"</f>
+        <v>Controller;</v>
+      </c>
+      <c r="V20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>20</v>
       </c>
@@ -1099,8 +1335,20 @@
       <c r="P21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U21" t="s">
+        <v>20</v>
+      </c>
+      <c r="V21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>10</v>
       </c>
@@ -1139,20 +1387,34 @@
         <f>O$18&amp;$C22&amp;O$19&amp;O$20</f>
         <v>NahkampfwaffeController.setHD(HD);</v>
       </c>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R22" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" t="str">
+        <f>R$18&amp;$C22&amp;R$19&amp;R$20</f>
+        <v>NahkampfwaffeController,</v>
+      </c>
+      <c r="U22" t="s">
+        <v>20</v>
+      </c>
+      <c r="V22" t="str">
+        <f>U$18&amp;$C22&amp;U$19&amp;LOWER($C22)&amp;U$20</f>
+        <v>NahkampfwaffeController = nahkampfwaffeController;</v>
+      </c>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ref="E23:E27" si="4">D$18&amp;$C23&amp;D$19&amp;$C23&amp;D$20</f>
+        <f t="shared" ref="E23:E27" si="6">D$18&amp;$C23&amp;D$19&amp;$C23&amp;D$20</f>
         <v>public CharController.Fernkampfwaffe FernkampfwaffeController { get; set; }</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" ref="G23:G29" si="5">F$18&amp;$C23&amp;F$19&amp;$C23&amp;F$20</f>
+        <f t="shared" ref="G23:G27" si="7">F$18&amp;$C23&amp;F$19&amp;$C23&amp;F$20</f>
         <v>FernkampfwaffeController = new CharController.Fernkampfwaffe();</v>
       </c>
       <c r="H23" t="s">
@@ -1162,37 +1424,51 @@
         <v>20</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:J27" si="6">I$18&amp;$C23&amp;I$19&amp;LOWER($C23)&amp;I$20</f>
+        <f t="shared" ref="J23:J27" si="8">I$18&amp;$C23&amp;I$19&amp;LOWER($C23)&amp;I$20</f>
         <v>FernkampfwaffeController = fernkampfwaffe;</v>
       </c>
       <c r="L23" t="s">
         <v>20</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" ref="M23:M27" si="7">L$18&amp;$C23&amp;L$19&amp;LOWER($C23)&amp;L$20</f>
+        <f t="shared" ref="M23:M27" si="9">L$18&amp;$C23&amp;L$19&amp;LOWER($C23)&amp;L$20</f>
         <v>CharController.Fernkampfwaffe fernkampfwaffe,</v>
       </c>
       <c r="O23" t="s">
         <v>20</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" ref="P23:P27" si="8">O$18&amp;$C23&amp;O$19&amp;O$20</f>
+        <f t="shared" ref="P23:P27" si="10">O$18&amp;$C23&amp;O$19&amp;O$20</f>
         <v>FernkampfwaffeController.setHD(HD);</v>
       </c>
-    </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" t="str">
+        <f t="shared" ref="S23:S27" si="11">R$18&amp;$C23&amp;R$19&amp;R$20</f>
+        <v>FernkampfwaffeController,</v>
+      </c>
+      <c r="U23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" ref="V23:V27" si="12">U$18&amp;$C23&amp;U$19&amp;LOWER($C23)&amp;U$20</f>
+        <v>FernkampfwaffeController = fernkampfwaffeController;</v>
+      </c>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public CharController.Kommlink KommlinkController { get; set; }</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>KommlinkController = new CharController.Kommlink();</v>
       </c>
       <c r="H24" t="s">
@@ -1202,37 +1478,51 @@
         <v>20</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>KommlinkController = kommlink;</v>
       </c>
       <c r="L24" t="s">
         <v>20</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>CharController.Kommlink kommlink,</v>
       </c>
       <c r="O24" t="s">
         <v>20</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>KommlinkController.setHD(HD);</v>
       </c>
-    </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R24" t="s">
+        <v>20</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" si="11"/>
+        <v>KommlinkController,</v>
+      </c>
+      <c r="U24" t="s">
+        <v>20</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="12"/>
+        <v>KommlinkController = kommlinkController;</v>
+      </c>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>15</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public CharController.CyberDeck CyberDeckController { get; set; }</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>CyberDeckController = new CharController.CyberDeck();</v>
       </c>
       <c r="H25" t="s">
@@ -1242,37 +1532,51 @@
         <v>20</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>CyberDeckController = cyberdeck;</v>
       </c>
       <c r="L25" t="s">
         <v>20</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>CharController.CyberDeck cyberdeck,</v>
       </c>
       <c r="O25" t="s">
         <v>20</v>
       </c>
       <c r="P25" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>CyberDeckController.setHD(HD);</v>
       </c>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="11"/>
+        <v>CyberDeckController,</v>
+      </c>
+      <c r="U25" t="s">
+        <v>20</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="12"/>
+        <v>CyberDeckController = cyberdeckController;</v>
+      </c>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public CharController.Vehikel VehikelController { get; set; }</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>VehikelController = new CharController.Vehikel();</v>
       </c>
       <c r="H26" t="s">
@@ -1282,37 +1586,51 @@
         <v>20</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>VehikelController = vehikel;</v>
       </c>
       <c r="L26" t="s">
         <v>20</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>CharController.Vehikel vehikel,</v>
       </c>
       <c r="O26" t="s">
         <v>20</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>VehikelController.setHD(HD);</v>
       </c>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>20</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" si="11"/>
+        <v>VehikelController,</v>
+      </c>
+      <c r="U26" t="s">
+        <v>20</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="12"/>
+        <v>VehikelController = vehikelController;</v>
+      </c>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>14</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>public CharController.Panzerung PanzerungController { get; set; }</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>PanzerungController = new CharController.Panzerung();</v>
       </c>
       <c r="H27" t="s">
@@ -1322,22 +1640,36 @@
         <v>20</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>PanzerungController = panzerung;</v>
       </c>
       <c r="L27" t="s">
         <v>20</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>CharController.Panzerung panzerung,</v>
       </c>
       <c r="O27" t="s">
         <v>20</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>PanzerungController.setHD(HD);</v>
+      </c>
+      <c r="R27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" t="str">
+        <f t="shared" si="11"/>
+        <v>PanzerungController,</v>
+      </c>
+      <c r="U27" t="s">
+        <v>20</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="12"/>
+        <v>PanzerungController = panzerungController;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>